<commit_message>
cleared errors course complete
</commit_message>
<xml_diff>
--- a/Datacamp Joining Data with Pandas/dji.xlsx
+++ b/Datacamp Joining Data with Pandas/dji.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanstevens/Documents/Python/Pandas/Joining Data with Pandas - Datacamp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jordanstevens/Documents/Python/Datacamp-Files-Git/Datacamp Joining Data with Pandas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA232ECA-A710-D142-88AF-83A9C308DA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87452B5-513F-1A46-97F8-C0AAECB550D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="940" yWindow="1700" windowWidth="25940" windowHeight="15260" xr2:uid="{AC3CC25B-DBAF-0440-800B-DE705DC1F4EC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>date</t>
   </si>
@@ -50,9 +50,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -82,9 +79,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,16 +400,13 @@
   <dimension ref="A1:B160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -422,1232 +417,1232 @@
       <c r="A2" s="1">
         <v>39114</v>
       </c>
-      <c r="B2">
-        <v>5.0000000000000001E-3</v>
+      <c r="B2" s="2">
+        <v>5.0939999999999996E-3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>39142</v>
       </c>
-      <c r="B3">
-        <v>-2.5999999999999999E-2</v>
+      <c r="B3" s="2">
+        <v>-2.614E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>39173</v>
       </c>
-      <c r="B4">
-        <v>4.9000000000000002E-2</v>
+      <c r="B4" s="2">
+        <v>4.8529999999999997E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>39203</v>
       </c>
-      <c r="B5">
-        <v>5.1999999999999998E-2</v>
+      <c r="B5" s="2">
+        <v>5.2010000000000001E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>39234</v>
       </c>
-      <c r="B6">
-        <v>-1.6E-2</v>
+      <c r="B6" s="2">
+        <v>-1.6070000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>39264</v>
       </c>
-      <c r="B7">
-        <v>2.3599999999999999E-2</v>
+      <c r="B7" s="2">
+        <v>3.8010000000000002E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>39295</v>
       </c>
-      <c r="B8">
-        <v>2.7199999999999998E-2</v>
+      <c r="B8" s="2">
+        <v>-6.3890000000000002E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>39326</v>
       </c>
-      <c r="B9">
-        <v>3.0800000000000001E-2</v>
+      <c r="B9" s="2">
+        <v>6.6519999999999996E-2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>39356</v>
       </c>
-      <c r="B10">
-        <v>3.44E-2</v>
+      <c r="B10" s="2">
+        <v>2.4759999999999999E-3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>39387</v>
       </c>
-      <c r="B11">
-        <v>3.7999999999999999E-2</v>
+      <c r="B11" s="2">
+        <v>-2.4039999999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>39417</v>
       </c>
-      <c r="B12">
-        <v>4.1599999999999998E-2</v>
+      <c r="B12" s="2">
+        <v>-1.0630000000000001E-2</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>39448</v>
       </c>
-      <c r="B13">
-        <v>4.5199999999999997E-2</v>
+      <c r="B13" s="2">
+        <v>-5.9490000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>39479</v>
       </c>
-      <c r="B14">
-        <v>4.8800000000000003E-2</v>
+      <c r="B14" s="2">
+        <v>-3.56E-2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>39508</v>
       </c>
-      <c r="B15">
-        <v>5.2400000000000002E-2</v>
+      <c r="B15" s="2">
+        <v>1.321E-2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>39539</v>
       </c>
-      <c r="B16">
-        <v>5.6000000000000001E-2</v>
+      <c r="B16" s="2">
+        <v>2.087E-2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>39569</v>
       </c>
-      <c r="B17">
-        <v>5.96E-2</v>
+      <c r="B17" s="2">
+        <v>-1.4339999999999999E-3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>39600</v>
       </c>
-      <c r="B18">
-        <v>6.3200000000000006E-2</v>
+      <c r="B18" s="2">
+        <v>-4.2700000000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>39630</v>
       </c>
-      <c r="B19">
-        <v>6.6799999999999998E-2</v>
+      <c r="B19" s="2">
+        <v>-5.74E-2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>39661</v>
       </c>
-      <c r="B20">
-        <v>7.0400000000000004E-2</v>
+      <c r="B20" s="2">
+        <v>2.5430000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>39692</v>
       </c>
-      <c r="B21">
-        <v>7.3999999999999996E-2</v>
+      <c r="B21" s="2">
+        <v>-6.9099999999999995E-2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>39722</v>
       </c>
-      <c r="B22">
-        <v>7.7600000000000002E-2</v>
+      <c r="B22" s="2">
+        <v>-0.1542</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>39753</v>
       </c>
-      <c r="B23">
-        <v>8.1199999999999994E-2</v>
+      <c r="B23" s="2">
+        <v>-8.0310000000000006E-2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>39783</v>
       </c>
-      <c r="B24">
-        <v>8.48E-2</v>
+      <c r="B24" s="2">
+        <v>5.8130000000000001E-2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>39814</v>
       </c>
-      <c r="B25">
-        <v>8.8400000000000006E-2</v>
+      <c r="B25" s="2">
+        <v>-3.7499999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>39845</v>
       </c>
-      <c r="B26">
-        <v>9.1999999999999998E-2</v>
+      <c r="B26" s="2">
+        <v>-0.1648</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>39873</v>
       </c>
-      <c r="B27">
-        <v>9.5600000000000004E-2</v>
+      <c r="B27" s="2">
+        <v>4.24E-2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>39904</v>
       </c>
-      <c r="B28">
-        <v>9.9199999999999997E-2</v>
+      <c r="B28" s="2">
+        <v>6.4509999999999998E-2</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>39934</v>
       </c>
-      <c r="B29">
-        <v>0.1028</v>
+      <c r="B29" s="2">
+        <v>5.6779999999999997E-2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>39965</v>
       </c>
-      <c r="B30">
-        <v>0.10639999999999999</v>
+      <c r="B30" s="2">
+        <v>3.8969999999999998E-2</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>39995</v>
       </c>
-      <c r="B31">
-        <v>0.11</v>
+      <c r="B31" s="2">
+        <v>-4.7829999999999998E-2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>40026</v>
       </c>
-      <c r="B32">
-        <v>0.11360000000000001</v>
+      <c r="B32" s="2">
+        <v>0.111</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>40057</v>
       </c>
-      <c r="B33">
-        <v>0.1172</v>
+      <c r="B33" s="2">
+        <v>5.7590000000000002E-2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>40087</v>
       </c>
-      <c r="B34">
-        <v>0.1208</v>
+      <c r="B34" s="2">
+        <v>-7.8279999999999999E-3</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>40118</v>
       </c>
-      <c r="B35">
-        <v>0.1244</v>
+      <c r="B35" s="2">
+        <v>7.739E-2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>40148</v>
       </c>
-      <c r="B36">
-        <v>0.128</v>
+      <c r="B36" s="2">
+        <v>-3.4780000000000002E-3</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>40179</v>
       </c>
-      <c r="B37">
-        <v>0.13159999999999999</v>
+      <c r="B37" s="2">
+        <v>-2.2409999999999999E-2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>40210</v>
       </c>
-      <c r="B38">
-        <v>0.13519999999999999</v>
+      <c r="B38" s="2">
+        <v>1.285E-2</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>40238</v>
       </c>
-      <c r="B39">
-        <v>0.13880000000000001</v>
+      <c r="B39" s="2">
+        <v>5.0860000000000002E-2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>40269</v>
       </c>
-      <c r="B40">
-        <v>0.1424</v>
+      <c r="B40" s="2">
+        <v>1.5509999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40299</v>
       </c>
-      <c r="B41">
-        <v>0.14599999999999999</v>
+      <c r="B41" s="2">
+        <v>-8.0049999999999996E-2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40330</v>
       </c>
-      <c r="B42">
-        <v>0.14960000000000001</v>
+      <c r="B42" s="2">
+        <v>-3.5770000000000003E-2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>40360</v>
       </c>
-      <c r="B43">
-        <v>0.1532</v>
+      <c r="B43" s="2">
+        <v>7.8130000000000005E-2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40391</v>
       </c>
-      <c r="B44">
-        <v>0.15679999999999999</v>
+      <c r="B44" s="2">
+        <v>-3.4479999999999997E-2</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>40422</v>
       </c>
-      <c r="B45">
-        <v>0.16039999999999999</v>
+      <c r="B45" s="2">
+        <v>6.7409999999999998E-2</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>40452</v>
       </c>
-      <c r="B46">
-        <v>0.16400000000000001</v>
+      <c r="B46" s="2">
+        <v>2.3769999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>40483</v>
       </c>
-      <c r="B47">
-        <v>0.1676</v>
+      <c r="B47" s="2">
+        <v>-2.3830000000000001E-3</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>40513</v>
       </c>
-      <c r="B48">
-        <v>0.17119999999999999</v>
+      <c r="B48" s="2">
+        <v>3.9780000000000003E-2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>40544</v>
       </c>
-      <c r="B49">
-        <v>0.17480000000000001</v>
+      <c r="B49" s="2">
+        <v>3.1099999999999999E-2</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>40575</v>
       </c>
-      <c r="B50">
-        <v>0.1784</v>
+      <c r="B50" s="2">
+        <v>1.4330000000000001E-2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>40603</v>
       </c>
-      <c r="B51">
-        <v>0.182</v>
+      <c r="B51" s="2">
+        <v>-2.1389999999999998E-3</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>40634</v>
       </c>
-      <c r="B52">
-        <v>0.18559999999999999</v>
+      <c r="B52" s="2">
+        <v>3.2419999999999997E-2</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>40664</v>
       </c>
-      <c r="B53">
-        <v>0.18920000000000001</v>
+      <c r="B53" s="2">
+        <v>1.199E-3</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>40695</v>
       </c>
-      <c r="B54">
-        <v>0.1928</v>
+      <c r="B54" s="2">
+        <v>-2.1940000000000002E-3</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>40725</v>
       </c>
-      <c r="B55">
-        <v>0.19639999999999999</v>
+      <c r="B55" s="2">
+        <v>2.6259999999999999E-3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>40756</v>
       </c>
-      <c r="B56">
-        <v>0.2</v>
+      <c r="B56" s="2">
+        <v>-6.6960000000000006E-2</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>40787</v>
       </c>
-      <c r="B57">
-        <v>0.2036</v>
+      <c r="B57" s="2">
+        <v>-3.6409999999999998E-2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>40817</v>
       </c>
-      <c r="B58">
-        <v>0.2072</v>
+      <c r="B58" s="2">
+        <v>2.5680000000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>40848</v>
       </c>
-      <c r="B59">
-        <v>0.21079999999999999</v>
+      <c r="B59" s="2">
+        <v>1.359E-3</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>40878</v>
       </c>
-      <c r="B60">
-        <v>0.21440000000000001</v>
+      <c r="B60" s="2">
+        <v>4.5909999999999999E-2</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>40909</v>
       </c>
-      <c r="B61">
-        <v>0.218</v>
+      <c r="B61" s="2">
+        <v>5.2600000000000001E-2</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>40940</v>
       </c>
-      <c r="B62">
-        <v>0.22159999999999999</v>
+      <c r="B62" s="2">
+        <v>1.7739999999999999E-2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>40969</v>
       </c>
-      <c r="B63">
-        <v>0.22520000000000001</v>
+      <c r="B63" s="2">
+        <v>2.5919999999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>41000</v>
       </c>
-      <c r="B64">
-        <v>0.2288</v>
+      <c r="B64" s="2">
+        <v>-9.1809999999999999E-3</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>41030</v>
       </c>
-      <c r="B65">
-        <v>0.2324</v>
+      <c r="B65" s="2">
+        <v>-5.3260000000000002E-2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>41061</v>
       </c>
-      <c r="B66">
-        <v>0.23599999999999999</v>
+      <c r="B66" s="2">
+        <v>3.4770000000000002E-2</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>41091</v>
       </c>
-      <c r="B67">
-        <v>0.23960000000000001</v>
+      <c r="B67" s="2">
+        <v>-1.404E-4</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>41122</v>
       </c>
-      <c r="B68">
-        <v>0.2432</v>
+      <c r="B68" s="2">
+        <v>3.5020000000000003E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>41153</v>
       </c>
-      <c r="B69">
-        <v>0.24679999999999999</v>
+      <c r="B69" s="2">
+        <v>2.4250000000000001E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>41183</v>
       </c>
-      <c r="B70">
-        <v>0.25040000000000001</v>
+      <c r="B70" s="2">
+        <v>-1.8270000000000002E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>41214</v>
       </c>
-      <c r="B71">
-        <v>0.254</v>
+      <c r="B71" s="2">
+        <v>-2.6970000000000001E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>41244</v>
       </c>
-      <c r="B72">
-        <v>0.2576</v>
+      <c r="B72" s="2">
+        <v>1.1860000000000001E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>41275</v>
       </c>
-      <c r="B73">
-        <v>0.26119999999999999</v>
+      <c r="B73" s="2">
+        <v>2.802E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>41306</v>
       </c>
-      <c r="B74">
-        <v>0.26479999999999998</v>
+      <c r="B74" s="2">
+        <v>3.6519999999999997E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>41334</v>
       </c>
-      <c r="B75">
-        <v>0.26840000000000003</v>
+      <c r="B75" s="2">
+        <v>2.349E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>41365</v>
       </c>
-      <c r="B76">
-        <v>0.27200000000000002</v>
+      <c r="B76" s="2">
+        <v>3.7379999999999997E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>41395</v>
       </c>
-      <c r="B77">
-        <v>0.27560000000000001</v>
+      <c r="B77" s="2">
+        <v>1.685E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>41426</v>
       </c>
-      <c r="B78">
-        <v>0.2792</v>
+      <c r="B78" s="2">
+        <v>-2.2489999999999999E-4</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>41456</v>
       </c>
-      <c r="B79">
-        <v>0.2828</v>
+      <c r="B79" s="2">
+        <v>2.563E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>41487</v>
       </c>
-      <c r="B80">
-        <v>0.28639999999999999</v>
+      <c r="B80" s="2">
+        <v>-4.249E-2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>41518</v>
       </c>
-      <c r="B81">
-        <v>0.28999999999999998</v>
+      <c r="B81" s="2">
+        <v>2.8119999999999999E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>41548</v>
       </c>
-      <c r="B82">
-        <v>0.29360000000000003</v>
+      <c r="B82" s="2">
+        <v>7.5760000000000003E-3</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>41579</v>
       </c>
-      <c r="B83">
-        <v>0.29720000000000002</v>
+      <c r="B83" s="2">
+        <v>3.2680000000000001E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>41609</v>
       </c>
-      <c r="B84">
-        <v>0.30080000000000001</v>
+      <c r="B84" s="2">
+        <v>1.8380000000000001E-2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>41640</v>
       </c>
-      <c r="B85">
-        <v>0.3044</v>
+      <c r="B85" s="2">
+        <v>1.5900000000000001E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>41671</v>
       </c>
-      <c r="B86">
-        <v>0.308</v>
+      <c r="B86" s="2">
+        <v>-1.494E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>41699</v>
       </c>
-      <c r="B87">
-        <v>0.31159999999999999</v>
+      <c r="B87" s="2">
+        <v>1.477E-2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>41730</v>
       </c>
-      <c r="B88">
-        <v>0.31519999999999998</v>
+      <c r="B88" s="2">
+        <v>7.1079999999999997E-3</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>41760</v>
       </c>
-      <c r="B89">
-        <v>0.31879999999999997</v>
+      <c r="B89" s="2">
+        <v>1.099E-2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>41791</v>
       </c>
-      <c r="B90">
-        <v>0.32240000000000002</v>
+      <c r="B90" s="2">
+        <v>6.5440000000000003E-3</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>41821</v>
       </c>
-      <c r="B91">
-        <v>0.32600000000000001</v>
+      <c r="B91" s="2">
+        <v>-0.99299999999999999</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>41852</v>
       </c>
-      <c r="B92">
-        <v>0.3296</v>
+      <c r="B92" s="2">
+        <v>144.5</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>41883</v>
       </c>
-      <c r="B93">
-        <v>0.3332</v>
+      <c r="B93" s="2">
+        <v>-3.2460000000000002E-3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>41913</v>
       </c>
-      <c r="B94">
-        <v>0.33679999999999999</v>
+      <c r="B94" s="2">
+        <v>2.0400000000000001E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>41944</v>
       </c>
-      <c r="B95">
-        <v>0.34039999999999998</v>
+      <c r="B95" s="2">
+        <v>2.5170000000000001E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>41974</v>
       </c>
-      <c r="B96">
-        <v>0.34399999999999997</v>
+      <c r="B96" s="2">
+        <v>-2.8600000000000001E-4</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>42005</v>
       </c>
-      <c r="B97">
-        <v>0.34760000000000002</v>
+      <c r="B97" s="2">
+        <v>-3.6929999999999998E-2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>42036</v>
       </c>
-      <c r="B98">
-        <v>0.35120000000000001</v>
+      <c r="B98" s="2">
+        <v>5.638E-2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>42064</v>
       </c>
-      <c r="B99">
-        <v>0.3548</v>
+      <c r="B99" s="2">
+        <v>-1.967E-2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>42095</v>
       </c>
-      <c r="B100">
-        <v>0.3584</v>
+      <c r="B100" s="2">
+        <v>1.4749999999999999E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>42125</v>
       </c>
-      <c r="B101">
-        <v>0.36199999999999999</v>
+      <c r="B101" s="2">
+        <v>-1.5299999999999999E-3</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>42156</v>
       </c>
-      <c r="B102">
-        <v>0.36559999999999998</v>
+      <c r="B102" s="2">
+        <v>-2.172E-2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>42186</v>
       </c>
-      <c r="B103">
-        <v>0.36919999999999997</v>
+      <c r="B103" s="2">
+        <v>6.3790000000000001E-3</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>42217</v>
       </c>
-      <c r="B104">
-        <v>0.37280000000000002</v>
+      <c r="B104" s="2">
+        <v>-6.7890000000000006E-2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>42248</v>
       </c>
-      <c r="B105">
-        <v>0.37640000000000001</v>
+      <c r="B105" s="2">
+        <v>-2.5749999999999999E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>42278</v>
       </c>
-      <c r="B106">
-        <v>0.38</v>
+      <c r="B106" s="2">
+        <v>9.6949999999999995E-2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>42309</v>
       </c>
-      <c r="B107">
-        <v>0.3836</v>
+      <c r="B107" s="2">
+        <v>3.1930000000000001E-3</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>42339</v>
       </c>
-      <c r="B108">
-        <v>0.38719999999999999</v>
+      <c r="B108" s="2">
+        <v>-1.6639999999999999E-2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>42370</v>
       </c>
-      <c r="B109">
-        <v>0.39079999999999998</v>
+      <c r="B109" s="2">
+        <v>-5.5019999999999999E-2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>42401</v>
       </c>
-      <c r="B110">
-        <v>0.39439999999999997</v>
+      <c r="B110" s="2">
+        <v>3.0490000000000001E-3</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>42430</v>
       </c>
-      <c r="B111">
-        <v>0.39800000000000002</v>
+      <c r="B111" s="2">
+        <v>7.0749999999999993E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>42461</v>
       </c>
-      <c r="B112">
-        <v>0.40160000000000001</v>
+      <c r="B112" s="2">
+        <v>5.0039999999999998E-3</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>42491</v>
       </c>
-      <c r="B113">
-        <v>0.4052</v>
+      <c r="B113" s="2">
+        <v>7.6519999999999995E-4</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>42522</v>
       </c>
-      <c r="B114">
-        <v>0.4088</v>
+      <c r="B114" s="2">
+        <v>8.0280000000000004E-3</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>42552</v>
       </c>
-      <c r="B115">
-        <v>0.41239999999999999</v>
+      <c r="B115" s="2">
+        <v>2.801E-2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>42583</v>
       </c>
-      <c r="B116">
-        <v>0.41599999999999998</v>
+      <c r="B116" s="2">
+        <v>-1.6980000000000001E-3</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>42614</v>
       </c>
-      <c r="B117">
-        <v>0.41959999999999997</v>
+      <c r="B117" s="2">
+        <v>-5.0379999999999999E-3</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>42644</v>
       </c>
-      <c r="B118">
-        <v>0.42320000000000002</v>
+      <c r="B118" s="2">
+        <v>-9.0559999999999998E-3</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>42675</v>
       </c>
-      <c r="B119">
-        <v>0.42680000000000001</v>
+      <c r="B119" s="2">
+        <v>5.4080000000000003E-2</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>42705</v>
       </c>
-      <c r="B120">
-        <v>0.4304</v>
+      <c r="B120" s="2">
+        <v>3.3410000000000002E-2</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>42736</v>
       </c>
-      <c r="B121">
-        <v>0.434</v>
+      <c r="B121" s="2">
+        <v>5.1359999999999999E-3</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>42767</v>
       </c>
-      <c r="B122">
-        <v>0.43759999999999999</v>
+      <c r="B122" s="2">
+        <v>4.7730000000000002E-2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>42795</v>
       </c>
-      <c r="B123">
-        <v>0.44119999999999998</v>
+      <c r="B123" s="2">
+        <v>-7.1590000000000004E-3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>42826</v>
       </c>
-      <c r="B124">
-        <v>0.44479999999999997</v>
+      <c r="B124" s="2">
+        <v>1.342E-2</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>42856</v>
       </c>
-      <c r="B125">
-        <v>0.44840000000000002</v>
+      <c r="B125" s="2">
+        <v>3.2569999999999999E-3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>42887</v>
       </c>
-      <c r="B126">
-        <v>0.45200000000000001</v>
+      <c r="B126" s="2">
+        <v>1.6230000000000001E-2</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>42917</v>
       </c>
-      <c r="B127">
-        <v>0.4556</v>
+      <c r="B127" s="2">
+        <v>2.5360000000000001E-2</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>42948</v>
       </c>
-      <c r="B128">
-        <v>0.4592</v>
+      <c r="B128" s="2">
+        <v>2.604E-3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>42979</v>
       </c>
-      <c r="B129">
-        <v>0.46279999999999999</v>
+      <c r="B129" s="2">
+        <v>2.0820000000000002E-2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>43009</v>
       </c>
-      <c r="B130">
-        <v>0.46639999999999998</v>
+      <c r="B130" s="2">
+        <v>4.3389999999999998E-2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>43040</v>
       </c>
-      <c r="B131">
-        <v>0.47</v>
+      <c r="B131" s="2">
+        <v>3.8289999999999998E-2</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>43070</v>
       </c>
-      <c r="B132">
-        <v>0.47360000000000002</v>
+      <c r="B132" s="2">
+        <v>1.8409999999999999E-2</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>43101</v>
       </c>
-      <c r="B133">
-        <v>0.47720000000000001</v>
+      <c r="B133" s="2">
+        <v>5.7860000000000002E-2</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>43132</v>
       </c>
-      <c r="B134">
-        <v>0.48080000000000001</v>
+      <c r="B134" s="2">
+        <v>-4.2840000000000003E-2</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>43160</v>
       </c>
-      <c r="B135">
-        <v>0.4844</v>
+      <c r="B135" s="2">
+        <v>-3.4660000000000003E-2</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>43191</v>
       </c>
-      <c r="B136">
-        <v>0.48799999999999999</v>
+      <c r="B136" s="2">
+        <v>6.2080000000000002E-5</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>43221</v>
       </c>
-      <c r="B137">
-        <v>0.49159999999999998</v>
+      <c r="B137" s="2">
+        <v>1.0460000000000001E-2</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>43252</v>
       </c>
-      <c r="B138">
-        <v>0.49519999999999997</v>
+      <c r="B138" s="2">
+        <v>-5.914E-3</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>43282</v>
       </c>
-      <c r="B139">
-        <v>0.49880000000000002</v>
+      <c r="B139" s="2">
+        <v>4.7129999999999998E-2</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>43313</v>
       </c>
-      <c r="B140">
-        <v>0.50239999999999996</v>
+      <c r="B140" s="2">
+        <v>2.162E-2</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>43344</v>
       </c>
-      <c r="B141">
-        <v>0.50600000000000001</v>
+      <c r="B141" s="2">
+        <v>1.9009999999999999E-2</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>43374</v>
       </c>
-      <c r="B142">
-        <v>0.50960000000000005</v>
+      <c r="B142" s="2">
+        <v>-5.074E-2</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>43405</v>
       </c>
-      <c r="B143">
-        <v>0.51319999999999999</v>
+      <c r="B143" s="2">
+        <v>1.6830000000000001E-2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>43435</v>
       </c>
-      <c r="B144">
-        <v>0.51680000000000004</v>
+      <c r="B144" s="2">
+        <v>-8.6580000000000004E-2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>43466</v>
       </c>
-      <c r="B145">
-        <v>0.52039999999999997</v>
+      <c r="B145" s="2">
+        <v>7.1679999999999994E-2</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>43497</v>
       </c>
-      <c r="B146">
-        <v>0.52400000000000002</v>
+      <c r="B146" s="2">
+        <v>3.6650000000000002E-2</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>43525</v>
       </c>
-      <c r="B147">
-        <v>0.52759999999999996</v>
+      <c r="B147" s="2">
+        <v>4.8999999999999998E-4</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>43556</v>
       </c>
-      <c r="B148">
-        <v>0.53120000000000001</v>
+      <c r="B148" s="2">
+        <v>2.562E-2</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>43586</v>
       </c>
-      <c r="B149">
-        <v>0.53480000000000005</v>
+      <c r="B149" s="2">
+        <v>-6.6860000000000003E-2</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>43617</v>
       </c>
-      <c r="B150">
-        <v>0.53839999999999999</v>
+      <c r="B150" s="2">
+        <v>7.8109999999999999E-2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>43647</v>
       </c>
-      <c r="B151">
-        <v>0.54200000000000004</v>
+      <c r="B151" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>43678</v>
       </c>
-      <c r="B152">
-        <v>0.54559999999999997</v>
+      <c r="B152" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>43709</v>
       </c>
-      <c r="B153">
-        <v>0.54920000000000002</v>
+      <c r="B153" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>43739</v>
       </c>
-      <c r="B154">
-        <v>0.55279999999999996</v>
+      <c r="B154" s="2">
+        <v>6.7790000000000003E-3</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>43770</v>
       </c>
-      <c r="B155">
-        <v>0.55640000000000001</v>
+      <c r="B155" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -1670,24 +1665,24 @@
       <c r="A158" s="1">
         <v>43862</v>
       </c>
-      <c r="B158">
-        <v>-0.01</v>
+      <c r="B158" s="2">
+        <v>-1.0449999999999999E-2</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>43891</v>
       </c>
-      <c r="B159">
-        <v>-0.216</v>
+      <c r="B159" s="2">
+        <v>-0.21609999999999999</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>43922</v>
       </c>
-      <c r="B160">
-        <v>3.5000000000000003E-2</v>
+      <c r="B160" s="2">
+        <v>3.4799999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>